<commit_message>
Deploying to gh-pages from  @ cf98bb7647bbc70cd3b5841180ae1eed0fd85079 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/10.4.1.xlsx
+++ b/en/downloads/data-excel/10.4.1.xlsx
@@ -530,7 +530,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0"/>
   </sheetViews>
@@ -542,7 +542,7 @@
     <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
@@ -553,7 +553,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>5</v>
       </c>
@@ -564,11 +564,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>6</v>
       </c>
@@ -608,8 +608,11 @@
       <c r="M4" s="10">
         <v>2019</v>
       </c>
+      <c r="N4" s="10">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
@@ -649,8 +652,11 @@
       <c r="M5" s="11">
         <v>24.5</v>
       </c>
+      <c r="N5" s="11">
+        <v>27.6</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 49525c58c1b0896b0dc263704bbe9f367bc557dd 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/10.4.1.xlsx
+++ b/en/downloads/data-excel/10.4.1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Наименование показателей</t>
   </si>
@@ -50,6 +50,74 @@
   </si>
   <si>
     <t>10.4.1 Жумушчулардын ИДПдагы кирешелеринин үлүшү, анын ичинде эмгек акы жана социалдык коргоо линиялары боюнча төлөмдөр</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> 2019-жылдан баштап маалыматтар, 2008 жылдагы Улуттук Эсептер Тутумунун эл аралык стандарттарына ылайык эсептелген </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">1 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Данные с 2019 года рассчитаны по международному стандарту Системы Национальных Счетов 2008 года</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> Data from 2019 are calculated according to the international standard of the System of National Accounts 2008</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -60,7 +128,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,6 +198,32 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <i/>
+      <vertAlign val="superscript"/>
+      <sz val="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial Cyr"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <vertAlign val="superscript"/>
+      <sz val="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -182,9 +276,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -192,11 +287,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -225,8 +315,18 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Normal_GDP1" xfId="2"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1"/>
   </cellStyles>
@@ -530,163 +630,171 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="42.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="39.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="37" style="2" customWidth="1"/>
+    <col min="1" max="3" width="36.7109375" style="2" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:17" ht="53.25" customHeight="1">
+      <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:17" ht="14.25" customHeight="1">
+      <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="14.25" customHeight="1" thickBot="1">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:17" ht="17.25" customHeight="1" thickBot="1">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="4">
         <v>2010</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="4">
         <v>2011</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="4">
         <v>2012</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="4">
         <v>2013</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="4">
         <v>2014</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="4">
         <v>2015</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="4">
         <v>2016</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="4">
         <v>2017</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="4">
         <v>2018</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="7">
         <v>2019</v>
       </c>
-      <c r="N4" s="10">
+      <c r="N4" s="7">
         <v>2020</v>
       </c>
-      <c r="O4" s="10">
+      <c r="O4" s="7">
         <v>2021</v>
       </c>
-      <c r="P4" s="10">
+      <c r="P4" s="7">
         <v>2022</v>
       </c>
+      <c r="Q4" s="7">
+        <v>2023</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:17" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="8">
         <v>29.6</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="9">
         <v>29</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="9">
         <v>30</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="8">
         <v>28.3</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="8">
         <v>26.8</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="9">
         <v>27</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="8">
         <v>28.4</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="8">
         <v>26.8</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="8">
         <v>26.1</v>
       </c>
-      <c r="M5" s="11">
+      <c r="M5" s="8">
         <v>23.2</v>
       </c>
-      <c r="N5" s="11">
+      <c r="N5" s="8">
         <v>25.8</v>
       </c>
-      <c r="O5" s="11">
+      <c r="O5" s="8">
         <v>24.1</v>
       </c>
-      <c r="P5" s="11">
+      <c r="P5" s="8">
         <v>24.5</v>
       </c>
+      <c r="Q5" s="8">
+        <v>23.4</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
+    <row r="6" spans="1:17" customFormat="1" ht="36" customHeight="1">
+      <c r="A6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>